<commit_message>
automatic update of 2022-09-21
</commit_message>
<xml_diff>
--- a/scripts/ESO-2.2m/schedules/P110/schedule-ESO-2.2m-P110.xlsx
+++ b/scripts/ESO-2.2m/schedules/P110/schedule-ESO-2.2m-P110.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="43">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -73,25 +73,25 @@
     <t xml:space="preserve">Hansen</t>
   </si>
   <si>
+    <t xml:space="preserve">Hobson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schinnerer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul, Sam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zakhozhay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul</t>
+  </si>
+  <si>
     <t xml:space="preserve">Downtime</t>
   </si>
   <si>
     <t xml:space="preserve">Recoating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schinnerer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul, Sam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zakhozhay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hobson</t>
   </si>
   <si>
     <t xml:space="preserve">Paul, Régis</t>
@@ -261,8 +261,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFB66C"/>
-        <bgColor rgb="FFFF99CC"/>
+        <fgColor rgb="FFFFDE59"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -306,7 +306,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -363,6 +363,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -376,19 +392,15 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -397,6 +409,10 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -477,7 +493,7 @@
       <rgbColor rgb="FFAFD095"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFB66C"/>
+      <rgbColor rgb="FFFFDE59"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -509,10 +525,10 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B173" activeCellId="0" sqref="B173"/>
+      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.17578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.78"/>
@@ -732,7 +748,7 @@
       <c r="B11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="12" t="s">
@@ -752,7 +768,7 @@
       <c r="B12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="12" t="s">
@@ -772,7 +788,7 @@
       <c r="B13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -792,7 +808,7 @@
       <c r="B14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="12" t="s">
@@ -812,7 +828,7 @@
       <c r="B15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="12" t="s">
@@ -832,8 +848,8 @@
       <c r="B16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>6</v>
+      <c r="C16" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>9</v>
@@ -852,8 +868,8 @@
       <c r="B17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>6</v>
+      <c r="C17" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>9</v>
@@ -870,15 +886,15 @@
         <v>44851</v>
       </c>
       <c r="B18" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="17"/>
+      <c r="E18" s="16"/>
       <c r="F18" s="7" t="s">
         <v>10</v>
       </c>
@@ -890,15 +906,15 @@
         <v>44852</v>
       </c>
       <c r="B19" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="17"/>
+      <c r="E19" s="16"/>
       <c r="F19" s="7" t="s">
         <v>10</v>
       </c>
@@ -910,15 +926,15 @@
         <v>44853</v>
       </c>
       <c r="B20" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="17"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="7" t="s">
         <v>10</v>
       </c>
@@ -930,15 +946,15 @@
         <v>44854</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="17"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="7" t="s">
         <v>10</v>
       </c>
@@ -950,15 +966,15 @@
         <v>44855</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="7" t="s">
         <v>10</v>
       </c>
@@ -972,13 +988,13 @@
       <c r="B23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>18</v>
+      <c r="C23" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="17"/>
       <c r="F23" s="7" t="s">
         <v>10</v>
       </c>
@@ -992,13 +1008,13 @@
       <c r="B24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>18</v>
+      <c r="C24" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="18"/>
+      <c r="E24" s="17"/>
       <c r="F24" s="7" t="s">
         <v>10</v>
       </c>
@@ -1012,13 +1028,13 @@
       <c r="B25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="18"/>
+      <c r="E25" s="17"/>
       <c r="F25" s="7" t="s">
         <v>10</v>
       </c>
@@ -1032,13 +1048,13 @@
       <c r="B26" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>18</v>
+      <c r="C26" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="18"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="7" t="s">
         <v>10</v>
       </c>
@@ -1052,13 +1068,13 @@
       <c r="B27" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>18</v>
+      <c r="C27" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="18"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="7" t="s">
         <v>10</v>
       </c>
@@ -1072,13 +1088,13 @@
       <c r="B28" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>21</v>
+      <c r="C28" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="18"/>
+      <c r="E28" s="17"/>
       <c r="F28" s="7" t="s">
         <v>10</v>
       </c>
@@ -1092,13 +1108,13 @@
       <c r="B29" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>21</v>
+      <c r="C29" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="7" t="s">
         <v>10</v>
       </c>
@@ -1112,13 +1128,13 @@
       <c r="B30" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>21</v>
+      <c r="C30" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="18"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="7" t="s">
         <v>10</v>
       </c>
@@ -1132,176 +1148,160 @@
       <c r="B31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>21</v>
+      <c r="C31" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="18"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="11" t="n">
+      <c r="A32" s="18" t="n">
         <f aca="false">A31+1</f>
         <v>44865</v>
       </c>
-      <c r="B32" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="12" t="s">
+      <c r="B32" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="C32" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22"/>
       <c r="G32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="19" t="n">
+      <c r="A33" s="23" t="n">
         <f aca="false">A32+1</f>
         <v>44866</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="12" t="s">
+      <c r="B33" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="C33" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
       <c r="G33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="19" t="n">
+      <c r="A34" s="23" t="n">
         <f aca="false">A33+1</f>
         <v>44867</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="12" t="s">
+      <c r="B34" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
       <c r="G34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="19" t="n">
+      <c r="A35" s="23" t="n">
         <f aca="false">A34+1</f>
         <v>44868</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="12" t="s">
+      <c r="B35" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
       <c r="G35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="19" t="n">
+      <c r="A36" s="23" t="n">
         <f aca="false">A35+1</f>
         <v>44869</v>
       </c>
-      <c r="B36" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="12" t="s">
+      <c r="B36" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E36" s="20"/>
-      <c r="F36" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
       <c r="G36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="19" t="n">
+      <c r="A37" s="23" t="n">
         <f aca="false">A36+1</f>
         <v>44870</v>
       </c>
-      <c r="B37" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="12" t="s">
+      <c r="B37" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
       <c r="G37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="11" t="n">
+      <c r="A38" s="18" t="n">
         <f aca="false">A37+1</f>
         <v>44871</v>
       </c>
-      <c r="B38" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="12" t="s">
+      <c r="B38" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="18"/>
-      <c r="F38" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E38" s="21"/>
+      <c r="F38" s="22"/>
       <c r="G38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="11" t="n">
+      <c r="A39" s="18" t="n">
         <f aca="false">A38+1</f>
         <v>44872</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="12" t="s">
+      <c r="B39" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E39" s="18"/>
-      <c r="F39" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E39" s="21"/>
+      <c r="F39" s="22"/>
       <c r="G39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1312,13 +1312,13 @@
       <c r="B40" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C40" s="12" t="s">
-        <v>22</v>
+      <c r="C40" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="18"/>
+      <c r="E40" s="17"/>
       <c r="F40" s="7" t="s">
         <v>10</v>
       </c>
@@ -1332,13 +1332,13 @@
       <c r="B41" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>22</v>
+      <c r="C41" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="18"/>
+      <c r="E41" s="17"/>
       <c r="F41" s="7" t="s">
         <v>10</v>
       </c>
@@ -1352,13 +1352,13 @@
       <c r="B42" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="12" t="s">
-        <v>22</v>
+      <c r="C42" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="18"/>
+      <c r="E42" s="17"/>
       <c r="F42" s="7" t="s">
         <v>10</v>
       </c>
@@ -1372,13 +1372,13 @@
       <c r="B43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="12" t="s">
-        <v>22</v>
+      <c r="C43" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="18"/>
+      <c r="E43" s="17"/>
       <c r="F43" s="7" t="s">
         <v>10</v>
       </c>
@@ -1392,13 +1392,13 @@
       <c r="B44" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>22</v>
+      <c r="C44" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E44" s="18"/>
+      <c r="E44" s="17"/>
       <c r="F44" s="7" t="s">
         <v>10</v>
       </c>
@@ -1412,13 +1412,13 @@
       <c r="B45" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>22</v>
+      <c r="C45" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="18"/>
+      <c r="E45" s="17"/>
       <c r="F45" s="7" t="s">
         <v>10</v>
       </c>
@@ -1432,13 +1432,13 @@
       <c r="B46" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>22</v>
+      <c r="C46" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E46" s="18"/>
+      <c r="E46" s="17"/>
       <c r="F46" s="7" t="s">
         <v>10</v>
       </c>
@@ -1452,13 +1452,13 @@
       <c r="B47" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C47" s="12" t="s">
-        <v>22</v>
+      <c r="C47" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E47" s="18"/>
+      <c r="E47" s="17"/>
       <c r="F47" s="7" t="s">
         <v>10</v>
       </c>
@@ -1472,13 +1472,13 @@
       <c r="B48" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>22</v>
+      <c r="C48" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="18"/>
+      <c r="E48" s="17"/>
       <c r="F48" s="7" t="s">
         <v>10</v>
       </c>
@@ -1492,13 +1492,13 @@
       <c r="B49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="12" t="s">
-        <v>22</v>
+      <c r="C49" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D49" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E49" s="18"/>
+      <c r="E49" s="17"/>
       <c r="F49" s="7" t="s">
         <v>10</v>
       </c>
@@ -1512,633 +1512,633 @@
       <c r="B50" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="12" t="s">
-        <v>22</v>
+      <c r="C50" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E50" s="18"/>
+      <c r="E50" s="17"/>
       <c r="F50" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="21" t="n">
+      <c r="A51" s="24" t="n">
         <f aca="false">A50+1</f>
         <v>44884</v>
       </c>
       <c r="B51" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="22"/>
+      <c r="E51" s="25"/>
       <c r="F51" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="21" t="n">
+      <c r="A52" s="24" t="n">
         <f aca="false">A51+1</f>
         <v>44885</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E52" s="22"/>
+      <c r="E52" s="25"/>
       <c r="F52" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="21" t="n">
+      <c r="A53" s="24" t="n">
         <f aca="false">A52+1</f>
         <v>44886</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E53" s="22"/>
+      <c r="E53" s="25"/>
       <c r="F53" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="21" t="n">
+      <c r="A54" s="24" t="n">
         <f aca="false">A53+1</f>
         <v>44887</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="22"/>
+      <c r="E54" s="25"/>
       <c r="F54" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="21" t="n">
+      <c r="A55" s="24" t="n">
         <f aca="false">A54+1</f>
         <v>44888</v>
       </c>
       <c r="B55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E55" s="22"/>
+      <c r="E55" s="25"/>
       <c r="F55" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="21" t="n">
+      <c r="A56" s="24" t="n">
         <f aca="false">A55+1</f>
         <v>44889</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C56" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E56" s="22"/>
+      <c r="E56" s="25"/>
       <c r="F56" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="21" t="n">
+      <c r="A57" s="24" t="n">
         <f aca="false">A56+1</f>
         <v>44890</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C57" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E57" s="22"/>
+      <c r="E57" s="25"/>
       <c r="F57" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="21" t="n">
+      <c r="A58" s="24" t="n">
         <f aca="false">A57+1</f>
         <v>44891</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C58" s="12" t="s">
+      <c r="C58" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E58" s="22"/>
+      <c r="E58" s="25"/>
       <c r="F58" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="21" t="n">
+      <c r="A59" s="24" t="n">
         <f aca="false">A58+1</f>
         <v>44892</v>
       </c>
       <c r="B59" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D59" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="22"/>
+      <c r="E59" s="25"/>
       <c r="F59" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="21" t="n">
+      <c r="A60" s="24" t="n">
         <f aca="false">A59+1</f>
         <v>44893</v>
       </c>
       <c r="B60" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E60" s="22"/>
+      <c r="E60" s="25"/>
       <c r="F60" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="21" t="n">
+      <c r="A61" s="24" t="n">
         <f aca="false">A60+1</f>
         <v>44894</v>
       </c>
       <c r="B61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D61" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E61" s="22"/>
+      <c r="E61" s="25"/>
       <c r="F61" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="21" t="n">
+      <c r="A62" s="24" t="n">
         <f aca="false">A61+1</f>
         <v>44895</v>
       </c>
       <c r="B62" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D62" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E62" s="22"/>
+      <c r="E62" s="25"/>
       <c r="F62" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="19" t="n">
+      <c r="A63" s="26" t="n">
         <f aca="false">A62+1</f>
         <v>44896</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E63" s="23"/>
+      <c r="E63" s="27"/>
       <c r="F63" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="19" t="n">
+      <c r="A64" s="26" t="n">
         <f aca="false">A63+1</f>
         <v>44897</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C64" s="12" t="s">
+      <c r="C64" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E64" s="23"/>
+      <c r="E64" s="27"/>
       <c r="F64" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="19" t="n">
+      <c r="A65" s="26" t="n">
         <f aca="false">A64+1</f>
         <v>44898</v>
       </c>
       <c r="B65" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C65" s="12" t="s">
+      <c r="C65" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D65" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E65" s="23"/>
+      <c r="E65" s="27"/>
       <c r="F65" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="19" t="n">
+      <c r="A66" s="26" t="n">
         <f aca="false">A65+1</f>
         <v>44899</v>
       </c>
       <c r="B66" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="C66" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E66" s="23"/>
+      <c r="E66" s="27"/>
       <c r="F66" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="19" t="n">
+      <c r="A67" s="26" t="n">
         <f aca="false">A66+1</f>
         <v>44900</v>
       </c>
       <c r="B67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C67" s="12" t="s">
+      <c r="C67" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D67" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E67" s="23"/>
+      <c r="E67" s="27"/>
       <c r="F67" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G67" s="8"/>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="19" t="n">
+      <c r="A68" s="26" t="n">
         <f aca="false">A67+1</f>
         <v>44901</v>
       </c>
       <c r="B68" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C68" s="12" t="s">
+      <c r="C68" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E68" s="23"/>
+      <c r="E68" s="27"/>
       <c r="F68" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G68" s="8"/>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="19" t="n">
+      <c r="A69" s="26" t="n">
         <f aca="false">A68+1</f>
         <v>44902</v>
       </c>
       <c r="B69" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="12" t="s">
+      <c r="C69" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D69" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E69" s="23"/>
+      <c r="E69" s="27"/>
       <c r="F69" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="19" t="n">
+      <c r="A70" s="26" t="n">
         <f aca="false">A69+1</f>
         <v>44903</v>
       </c>
       <c r="B70" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C70" s="12" t="s">
+      <c r="C70" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D70" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E70" s="23"/>
+      <c r="E70" s="27"/>
       <c r="F70" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G70" s="8"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="19" t="n">
+      <c r="A71" s="26" t="n">
         <f aca="false">A70+1</f>
         <v>44904</v>
       </c>
       <c r="B71" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C71" s="12" t="s">
+      <c r="C71" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D71" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E71" s="23"/>
+      <c r="E71" s="27"/>
       <c r="F71" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G71" s="8"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="19" t="n">
+      <c r="A72" s="26" t="n">
         <f aca="false">A71+1</f>
         <v>44905</v>
       </c>
       <c r="B72" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C72" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E72" s="23"/>
+      <c r="E72" s="27"/>
       <c r="F72" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="19" t="n">
+      <c r="A73" s="26" t="n">
         <f aca="false">A72+1</f>
         <v>44906</v>
       </c>
       <c r="B73" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C73" s="12" t="s">
+      <c r="C73" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D73" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E73" s="23"/>
+      <c r="E73" s="27"/>
       <c r="F73" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G73" s="8"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="19" t="n">
+      <c r="A74" s="26" t="n">
         <f aca="false">A73+1</f>
         <v>44907</v>
       </c>
       <c r="B74" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C74" s="12" t="s">
+      <c r="C74" s="0" t="s">
         <v>27</v>
       </c>
       <c r="D74" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E74" s="23"/>
+      <c r="E74" s="27"/>
       <c r="F74" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G74" s="8"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="19" t="n">
+      <c r="A75" s="26" t="n">
         <f aca="false">A74+1</f>
         <v>44908</v>
       </c>
       <c r="B75" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C75" s="12" t="s">
-        <v>22</v>
+      <c r="C75" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D75" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E75" s="23"/>
+      <c r="E75" s="27"/>
       <c r="F75" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="19" t="n">
+      <c r="A76" s="26" t="n">
         <f aca="false">A75+1</f>
         <v>44909</v>
       </c>
       <c r="B76" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C76" s="12" t="s">
-        <v>22</v>
+      <c r="C76" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D76" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E76" s="23"/>
+      <c r="E76" s="27"/>
       <c r="F76" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G76" s="8"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="19" t="n">
+      <c r="A77" s="26" t="n">
         <f aca="false">A76+1</f>
         <v>44910</v>
       </c>
       <c r="B77" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C77" s="12" t="s">
-        <v>22</v>
+      <c r="C77" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D77" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E77" s="23"/>
+      <c r="E77" s="27"/>
       <c r="F77" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G77" s="8"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="19" t="n">
+      <c r="A78" s="26" t="n">
         <f aca="false">A77+1</f>
         <v>44911</v>
       </c>
       <c r="B78" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C78" s="12" t="s">
-        <v>22</v>
+      <c r="C78" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D78" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E78" s="23"/>
+      <c r="E78" s="27"/>
       <c r="F78" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G78" s="8"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="19" t="n">
+      <c r="A79" s="26" t="n">
         <f aca="false">A78+1</f>
         <v>44912</v>
       </c>
       <c r="B79" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C79" s="12" t="s">
-        <v>22</v>
+      <c r="C79" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D79" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E79" s="23"/>
+      <c r="E79" s="27"/>
       <c r="F79" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G79" s="8"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="19" t="n">
+      <c r="A80" s="26" t="n">
         <f aca="false">A79+1</f>
         <v>44913</v>
       </c>
       <c r="B80" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="12" t="s">
-        <v>22</v>
+      <c r="C80" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D80" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E80" s="23"/>
+      <c r="E80" s="27"/>
       <c r="F80" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G80" s="8"/>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="19" t="n">
+      <c r="A81" s="26" t="n">
         <f aca="false">A80+1</f>
         <v>44914</v>
       </c>
       <c r="B81" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="12" t="s">
+      <c r="C81" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D81" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E81" s="23"/>
+      <c r="E81" s="27"/>
       <c r="F81" s="7" t="s">
         <v>10</v>
       </c>
@@ -2152,13 +2152,13 @@
       <c r="B82" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C82" s="12" t="s">
+      <c r="C82" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D82" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E82" s="18"/>
+      <c r="E82" s="17"/>
       <c r="F82" s="7" t="s">
         <v>10</v>
       </c>
@@ -2172,13 +2172,13 @@
       <c r="B83" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C83" s="12" t="s">
+      <c r="C83" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D83" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E83" s="18"/>
+      <c r="E83" s="17"/>
       <c r="F83" s="7" t="s">
         <v>10</v>
       </c>
@@ -2192,13 +2192,13 @@
       <c r="B84" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C84" s="12" t="s">
+      <c r="C84" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D84" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E84" s="18"/>
+      <c r="E84" s="17"/>
       <c r="F84" s="7" t="s">
         <v>10</v>
       </c>
@@ -2212,13 +2212,13 @@
       <c r="B85" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="C85" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D85" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E85" s="18"/>
+      <c r="E85" s="17"/>
       <c r="F85" s="7" t="s">
         <v>10</v>
       </c>
@@ -2232,253 +2232,253 @@
       <c r="B86" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C86" s="12" t="s">
+      <c r="C86" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D86" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E86" s="18"/>
+      <c r="E86" s="17"/>
       <c r="F86" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G86" s="8"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="19" t="n">
+      <c r="A87" s="26" t="n">
         <f aca="false">A86+1</f>
         <v>44920</v>
       </c>
       <c r="B87" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C87" s="12" t="s">
+      <c r="C87" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D87" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E87" s="18"/>
+      <c r="E87" s="17"/>
       <c r="F87" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G87" s="8"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="19" t="n">
+      <c r="A88" s="26" t="n">
         <f aca="false">A87+1</f>
         <v>44921</v>
       </c>
       <c r="B88" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C88" s="12" t="s">
-        <v>22</v>
+      <c r="C88" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D88" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E88" s="18"/>
+      <c r="E88" s="17"/>
       <c r="F88" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G88" s="8"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="19" t="n">
+      <c r="A89" s="26" t="n">
         <f aca="false">A88+1</f>
         <v>44922</v>
       </c>
       <c r="B89" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C89" s="12" t="s">
-        <v>22</v>
+      <c r="C89" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D89" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E89" s="18"/>
+      <c r="E89" s="17"/>
       <c r="F89" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G89" s="8"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="19" t="n">
+      <c r="A90" s="26" t="n">
         <f aca="false">A89+1</f>
         <v>44923</v>
       </c>
       <c r="B90" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C90" s="12" t="s">
-        <v>22</v>
+      <c r="C90" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D90" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E90" s="18"/>
+      <c r="E90" s="17"/>
       <c r="F90" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G90" s="8"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="19" t="n">
+      <c r="A91" s="26" t="n">
         <f aca="false">A90+1</f>
         <v>44924</v>
       </c>
       <c r="B91" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C91" s="12" t="s">
-        <v>22</v>
+      <c r="C91" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D91" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E91" s="18"/>
+      <c r="E91" s="17"/>
       <c r="F91" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G91" s="8"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="19" t="n">
+      <c r="A92" s="26" t="n">
         <f aca="false">A91+1</f>
         <v>44925</v>
       </c>
       <c r="B92" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C92" s="12" t="s">
-        <v>22</v>
+      <c r="C92" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D92" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E92" s="18"/>
+      <c r="E92" s="17"/>
       <c r="F92" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G92" s="8"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="19" t="n">
+      <c r="A93" s="26" t="n">
         <f aca="false">A92+1</f>
         <v>44926</v>
       </c>
       <c r="B93" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C93" s="12" t="s">
-        <v>22</v>
+      <c r="C93" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D93" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E93" s="18"/>
+      <c r="E93" s="17"/>
       <c r="F93" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G93" s="8"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="19" t="n">
+      <c r="A94" s="26" t="n">
         <f aca="false">A93+1</f>
         <v>44927</v>
       </c>
       <c r="B94" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C94" s="12" t="s">
-        <v>22</v>
+      <c r="C94" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D94" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E94" s="18"/>
+      <c r="E94" s="17"/>
       <c r="F94" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G94" s="8"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="19" t="n">
+      <c r="A95" s="26" t="n">
         <f aca="false">A94+1</f>
         <v>44928</v>
       </c>
       <c r="B95" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C95" s="12" t="s">
-        <v>22</v>
+      <c r="C95" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D95" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E95" s="18"/>
+      <c r="E95" s="17"/>
       <c r="F95" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G95" s="8"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="19" t="n">
+      <c r="A96" s="26" t="n">
         <f aca="false">A95+1</f>
         <v>44929</v>
       </c>
       <c r="B96" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C96" s="12" t="s">
-        <v>22</v>
+      <c r="C96" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="D96" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E96" s="18"/>
+      <c r="E96" s="17"/>
       <c r="F96" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G96" s="8"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="19" t="n">
+      <c r="A97" s="26" t="n">
         <f aca="false">A96+1</f>
         <v>44930</v>
       </c>
       <c r="B97" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C97" s="12" t="s">
+      <c r="C97" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D97" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E97" s="18"/>
+      <c r="E97" s="17"/>
       <c r="F97" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G97" s="8"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="19" t="n">
+      <c r="A98" s="26" t="n">
         <f aca="false">A97+1</f>
         <v>44931</v>
       </c>
       <c r="B98" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C98" s="12" t="s">
+      <c r="C98" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D98" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E98" s="18"/>
+      <c r="E98" s="17"/>
       <c r="F98" s="7" t="s">
         <v>10</v>
       </c>
@@ -2492,13 +2492,13 @@
       <c r="B99" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C99" s="12" t="s">
+      <c r="C99" s="0" t="s">
         <v>30</v>
       </c>
       <c r="D99" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E99" s="24"/>
+      <c r="E99" s="28"/>
       <c r="F99" s="7" t="s">
         <v>10</v>
       </c>
@@ -2518,7 +2518,7 @@
       <c r="D100" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E100" s="25"/>
+      <c r="E100" s="29"/>
       <c r="F100" s="7" t="s">
         <v>10</v>
       </c>
@@ -2538,7 +2538,7 @@
       <c r="D101" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E101" s="25"/>
+      <c r="E101" s="29"/>
       <c r="F101" s="7" t="s">
         <v>10</v>
       </c>
@@ -2558,7 +2558,7 @@
       <c r="D102" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E102" s="25"/>
+      <c r="E102" s="29"/>
       <c r="F102" s="7" t="s">
         <v>10</v>
       </c>
@@ -2578,187 +2578,187 @@
       <c r="D103" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E103" s="25"/>
+      <c r="E103" s="29"/>
       <c r="F103" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G103" s="8"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="26" t="n">
+      <c r="A104" s="30" t="n">
         <f aca="false">A103+1</f>
         <v>44937</v>
       </c>
-      <c r="B104" s="27" t="s">
+      <c r="B104" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C104" s="27"/>
-      <c r="D104" s="27" t="s">
+      <c r="C104" s="31"/>
+      <c r="D104" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E104" s="28"/>
+      <c r="E104" s="32"/>
       <c r="F104" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G104" s="8"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="26" t="n">
+      <c r="A105" s="30" t="n">
         <f aca="false">A104+1</f>
         <v>44938</v>
       </c>
-      <c r="B105" s="27" t="s">
+      <c r="B105" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C105" s="27"/>
-      <c r="D105" s="27" t="s">
+      <c r="C105" s="31"/>
+      <c r="D105" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E105" s="28"/>
+      <c r="E105" s="32"/>
       <c r="F105" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G105" s="8"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="26" t="n">
+      <c r="A106" s="30" t="n">
         <f aca="false">A105+1</f>
         <v>44939</v>
       </c>
-      <c r="B106" s="27" t="s">
+      <c r="B106" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C106" s="27"/>
-      <c r="D106" s="27" t="s">
+      <c r="C106" s="31"/>
+      <c r="D106" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E106" s="28"/>
+      <c r="E106" s="32"/>
       <c r="F106" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G106" s="8"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="26" t="n">
+      <c r="A107" s="30" t="n">
         <f aca="false">A106+1</f>
         <v>44940</v>
       </c>
-      <c r="B107" s="27" t="s">
+      <c r="B107" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C107" s="27"/>
-      <c r="D107" s="27" t="s">
+      <c r="C107" s="31"/>
+      <c r="D107" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E107" s="28"/>
+      <c r="E107" s="32"/>
       <c r="F107" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G107" s="8"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="26" t="n">
+      <c r="A108" s="30" t="n">
         <f aca="false">A107+1</f>
         <v>44941</v>
       </c>
-      <c r="B108" s="27" t="s">
+      <c r="B108" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27" t="s">
+      <c r="C108" s="31"/>
+      <c r="D108" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E108" s="28"/>
+      <c r="E108" s="32"/>
       <c r="F108" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G108" s="8"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="26" t="n">
+      <c r="A109" s="30" t="n">
         <f aca="false">A108+1</f>
         <v>44942</v>
       </c>
-      <c r="B109" s="27" t="s">
+      <c r="B109" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C109" s="27"/>
-      <c r="D109" s="27" t="s">
+      <c r="C109" s="31"/>
+      <c r="D109" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E109" s="28"/>
+      <c r="E109" s="32"/>
       <c r="F109" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G109" s="8"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="26" t="n">
+      <c r="A110" s="30" t="n">
         <f aca="false">A109+1</f>
         <v>44943</v>
       </c>
-      <c r="B110" s="27" t="s">
+      <c r="B110" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C110" s="27"/>
-      <c r="D110" s="27" t="s">
+      <c r="C110" s="31"/>
+      <c r="D110" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E110" s="28"/>
+      <c r="E110" s="32"/>
       <c r="F110" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G110" s="8"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="26" t="n">
+      <c r="A111" s="30" t="n">
         <f aca="false">A110+1</f>
         <v>44944</v>
       </c>
-      <c r="B111" s="27" t="s">
+      <c r="B111" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C111" s="27"/>
-      <c r="D111" s="27" t="s">
+      <c r="C111" s="31"/>
+      <c r="D111" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E111" s="28"/>
+      <c r="E111" s="32"/>
       <c r="F111" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G111" s="8"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="26" t="n">
+      <c r="A112" s="30" t="n">
         <f aca="false">A111+1</f>
         <v>44945</v>
       </c>
-      <c r="B112" s="27" t="s">
+      <c r="B112" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C112" s="27"/>
-      <c r="D112" s="27" t="s">
+      <c r="C112" s="31"/>
+      <c r="D112" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E112" s="28"/>
+      <c r="E112" s="32"/>
       <c r="F112" s="7" t="s">
         <v>10</v>
       </c>
       <c r="G112" s="8"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="26" t="n">
+      <c r="A113" s="30" t="n">
         <f aca="false">A112+1</f>
         <v>44946</v>
       </c>
-      <c r="B113" s="27" t="s">
+      <c r="B113" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27" t="s">
+      <c r="C113" s="31"/>
+      <c r="D113" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E113" s="28"/>
+      <c r="E113" s="32"/>
       <c r="F113" s="7" t="s">
         <v>10</v>
       </c>
@@ -2773,12 +2773,12 @@
         <v>14</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D114" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E114" s="24"/>
+      <c r="E114" s="28"/>
       <c r="F114" s="7" t="s">
         <v>10</v>
       </c>
@@ -2793,12 +2793,12 @@
         <v>14</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D115" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E115" s="24"/>
+      <c r="E115" s="28"/>
       <c r="F115" s="7" t="s">
         <v>10</v>
       </c>
@@ -2813,12 +2813,12 @@
         <v>14</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D116" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E116" s="24"/>
+      <c r="E116" s="28"/>
       <c r="F116" s="7" t="s">
         <v>10</v>
       </c>
@@ -2833,12 +2833,12 @@
         <v>14</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D117" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E117" s="24"/>
+      <c r="E117" s="28"/>
       <c r="F117" s="7" t="s">
         <v>10</v>
       </c>
@@ -2853,12 +2853,12 @@
         <v>14</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D118" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E118" s="24"/>
+      <c r="E118" s="28"/>
       <c r="F118" s="7" t="s">
         <v>10</v>
       </c>
@@ -2873,12 +2873,12 @@
         <v>14</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D119" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E119" s="24"/>
+      <c r="E119" s="28"/>
       <c r="F119" s="7" t="s">
         <v>10</v>
       </c>
@@ -2893,12 +2893,12 @@
         <v>14</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D120" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E120" s="24"/>
+      <c r="E120" s="28"/>
       <c r="F120" s="7" t="s">
         <v>10</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="D121" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E121" s="24"/>
+      <c r="E121" s="28"/>
       <c r="F121" s="7" t="s">
         <v>10</v>
       </c>
@@ -2938,7 +2938,7 @@
       <c r="D122" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E122" s="24"/>
+      <c r="E122" s="28"/>
       <c r="F122" s="7" t="s">
         <v>10</v>
       </c>
@@ -2958,7 +2958,7 @@
       <c r="D123" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E123" s="24"/>
+      <c r="E123" s="28"/>
       <c r="F123" s="7" t="s">
         <v>10</v>
       </c>
@@ -2978,7 +2978,7 @@
       <c r="D124" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E124" s="24"/>
+      <c r="E124" s="28"/>
       <c r="F124" s="7" t="s">
         <v>10</v>
       </c>
@@ -2998,7 +2998,7 @@
       <c r="D125" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E125" s="24"/>
+      <c r="E125" s="28"/>
       <c r="F125" s="7" t="s">
         <v>10</v>
       </c>
@@ -3018,7 +3018,7 @@
       <c r="D126" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E126" s="24"/>
+      <c r="E126" s="28"/>
       <c r="F126" s="7" t="s">
         <v>10</v>
       </c>
@@ -3038,7 +3038,7 @@
       <c r="D127" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E127" s="24"/>
+      <c r="E127" s="28"/>
       <c r="F127" s="7" t="s">
         <v>10</v>
       </c>
@@ -3058,7 +3058,7 @@
       <c r="D128" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E128" s="24"/>
+      <c r="E128" s="28"/>
       <c r="F128" s="7" t="s">
         <v>10</v>
       </c>
@@ -3078,7 +3078,7 @@
       <c r="D129" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E129" s="24"/>
+      <c r="E129" s="28"/>
       <c r="F129" s="7" t="s">
         <v>10</v>
       </c>
@@ -3098,7 +3098,7 @@
       <c r="D130" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E130" s="24"/>
+      <c r="E130" s="28"/>
       <c r="F130" s="7" t="s">
         <v>10</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="D131" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E131" s="24"/>
+      <c r="E131" s="28"/>
       <c r="F131" s="7" t="s">
         <v>10</v>
       </c>
@@ -3138,7 +3138,7 @@
       <c r="D132" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E132" s="24"/>
+      <c r="E132" s="28"/>
       <c r="F132" s="7" t="s">
         <v>10</v>
       </c>
@@ -3158,7 +3158,7 @@
       <c r="D133" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E133" s="24"/>
+      <c r="E133" s="28"/>
       <c r="F133" s="7" t="s">
         <v>10</v>
       </c>
@@ -3178,7 +3178,7 @@
       <c r="D134" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E134" s="24"/>
+      <c r="E134" s="28"/>
       <c r="F134" s="7" t="s">
         <v>10</v>
       </c>
@@ -3198,7 +3198,7 @@
       <c r="D135" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E135" s="24"/>
+      <c r="E135" s="28"/>
       <c r="F135" s="7" t="s">
         <v>10</v>
       </c>
@@ -3218,7 +3218,7 @@
       <c r="D136" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E136" s="24"/>
+      <c r="E136" s="28"/>
       <c r="F136" s="7" t="s">
         <v>10</v>
       </c>
@@ -3238,7 +3238,7 @@
       <c r="D137" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E137" s="24"/>
+      <c r="E137" s="28"/>
       <c r="F137" s="7" t="s">
         <v>10</v>
       </c>
@@ -3258,7 +3258,7 @@
       <c r="D138" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E138" s="24"/>
+      <c r="E138" s="28"/>
       <c r="F138" s="7" t="s">
         <v>10</v>
       </c>
@@ -3278,7 +3278,7 @@
       <c r="D139" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E139" s="24"/>
+      <c r="E139" s="28"/>
       <c r="F139" s="7" t="s">
         <v>10</v>
       </c>
@@ -3298,7 +3298,7 @@
       <c r="D140" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E140" s="24"/>
+      <c r="E140" s="28"/>
       <c r="F140" s="7" t="s">
         <v>10</v>
       </c>
@@ -3318,7 +3318,7 @@
       <c r="D141" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E141" s="24"/>
+      <c r="E141" s="28"/>
       <c r="F141" s="7" t="s">
         <v>10</v>
       </c>
@@ -3338,7 +3338,7 @@
       <c r="D142" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E142" s="24"/>
+      <c r="E142" s="28"/>
       <c r="F142" s="7" t="s">
         <v>10</v>
       </c>
@@ -3358,7 +3358,7 @@
       <c r="D143" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E143" s="24"/>
+      <c r="E143" s="28"/>
       <c r="F143" s="7" t="s">
         <v>10</v>
       </c>
@@ -3378,7 +3378,7 @@
       <c r="D144" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E144" s="24"/>
+      <c r="E144" s="28"/>
       <c r="F144" s="7" t="s">
         <v>10</v>
       </c>
@@ -3398,7 +3398,7 @@
       <c r="D145" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E145" s="24"/>
+      <c r="E145" s="28"/>
       <c r="F145" s="7" t="s">
         <v>10</v>
       </c>
@@ -3418,7 +3418,7 @@
       <c r="D146" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E146" s="24"/>
+      <c r="E146" s="28"/>
       <c r="F146" s="7" t="s">
         <v>10</v>
       </c>
@@ -3438,7 +3438,7 @@
       <c r="D147" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E147" s="24"/>
+      <c r="E147" s="28"/>
       <c r="F147" s="7" t="s">
         <v>10</v>
       </c>
@@ -3458,7 +3458,7 @@
       <c r="D148" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E148" s="24"/>
+      <c r="E148" s="28"/>
       <c r="F148" s="7" t="s">
         <v>10</v>
       </c>
@@ -3478,7 +3478,7 @@
       <c r="D149" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E149" s="24"/>
+      <c r="E149" s="28"/>
       <c r="F149" s="7" t="s">
         <v>10</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="D150" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E150" s="24"/>
+      <c r="E150" s="28"/>
       <c r="F150" s="7" t="s">
         <v>10</v>
       </c>
@@ -3518,7 +3518,7 @@
       <c r="D151" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E151" s="24"/>
+      <c r="E151" s="28"/>
       <c r="F151" s="7" t="s">
         <v>10</v>
       </c>
@@ -3538,7 +3538,7 @@
       <c r="D152" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E152" s="24"/>
+      <c r="E152" s="28"/>
       <c r="F152" s="7" t="s">
         <v>10</v>
       </c>
@@ -3558,7 +3558,7 @@
       <c r="D153" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E153" s="24"/>
+      <c r="E153" s="28"/>
       <c r="F153" s="7" t="s">
         <v>10</v>
       </c>
@@ -3578,7 +3578,7 @@
       <c r="D154" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E154" s="24"/>
+      <c r="E154" s="28"/>
       <c r="F154" s="7" t="s">
         <v>10</v>
       </c>
@@ -3598,7 +3598,7 @@
       <c r="D155" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E155" s="24"/>
+      <c r="E155" s="28"/>
       <c r="F155" s="7" t="s">
         <v>10</v>
       </c>
@@ -3618,7 +3618,7 @@
       <c r="D156" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E156" s="24"/>
+      <c r="E156" s="28"/>
       <c r="F156" s="7" t="s">
         <v>10</v>
       </c>
@@ -3638,7 +3638,7 @@
       <c r="D157" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E157" s="24"/>
+      <c r="E157" s="28"/>
       <c r="F157" s="7" t="s">
         <v>10</v>
       </c>
@@ -3658,7 +3658,7 @@
       <c r="D158" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E158" s="24"/>
+      <c r="E158" s="28"/>
       <c r="F158" s="7" t="s">
         <v>10</v>
       </c>
@@ -3678,7 +3678,7 @@
       <c r="D159" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E159" s="24"/>
+      <c r="E159" s="28"/>
       <c r="F159" s="7" t="s">
         <v>10</v>
       </c>
@@ -3698,7 +3698,7 @@
       <c r="D160" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E160" s="24"/>
+      <c r="E160" s="28"/>
       <c r="F160" s="7" t="s">
         <v>10</v>
       </c>
@@ -3718,7 +3718,7 @@
       <c r="D161" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E161" s="24"/>
+      <c r="E161" s="28"/>
       <c r="F161" s="7" t="s">
         <v>10</v>
       </c>
@@ -3738,7 +3738,7 @@
       <c r="D162" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E162" s="24"/>
+      <c r="E162" s="28"/>
       <c r="F162" s="7" t="s">
         <v>10</v>
       </c>
@@ -3758,7 +3758,7 @@
       <c r="D163" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E163" s="24"/>
+      <c r="E163" s="28"/>
       <c r="F163" s="7" t="s">
         <v>10</v>
       </c>
@@ -3778,7 +3778,7 @@
       <c r="D164" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E164" s="24"/>
+      <c r="E164" s="28"/>
       <c r="F164" s="7" t="s">
         <v>10</v>
       </c>
@@ -3798,7 +3798,7 @@
       <c r="D165" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E165" s="24"/>
+      <c r="E165" s="28"/>
       <c r="F165" s="7" t="s">
         <v>10</v>
       </c>
@@ -3818,7 +3818,7 @@
       <c r="D166" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E166" s="24"/>
+      <c r="E166" s="28"/>
       <c r="F166" s="7" t="s">
         <v>10</v>
       </c>
@@ -3838,7 +3838,7 @@
       <c r="D167" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E167" s="24"/>
+      <c r="E167" s="28"/>
       <c r="F167" s="7" t="s">
         <v>10</v>
       </c>
@@ -3858,7 +3858,7 @@
       <c r="D168" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E168" s="24"/>
+      <c r="E168" s="28"/>
       <c r="F168" s="7" t="s">
         <v>10</v>
       </c>
@@ -3873,12 +3873,12 @@
         <v>14</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D169" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E169" s="24"/>
+      <c r="E169" s="28"/>
       <c r="F169" s="7" t="s">
         <v>10</v>
       </c>
@@ -3893,12 +3893,12 @@
         <v>14</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D170" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E170" s="24"/>
+      <c r="E170" s="28"/>
       <c r="F170" s="7" t="s">
         <v>10</v>
       </c>
@@ -3913,12 +3913,12 @@
         <v>14</v>
       </c>
       <c r="C171" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D171" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E171" s="24"/>
+      <c r="E171" s="28"/>
       <c r="F171" s="7" t="s">
         <v>10</v>
       </c>
@@ -3933,12 +3933,12 @@
         <v>14</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D172" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E172" s="24"/>
+      <c r="E172" s="28"/>
       <c r="F172" s="7" t="s">
         <v>10</v>
       </c>
@@ -3958,7 +3958,7 @@
       <c r="D173" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E173" s="29"/>
+      <c r="E173" s="33"/>
       <c r="F173" s="7" t="s">
         <v>10</v>
       </c>
@@ -3978,7 +3978,7 @@
       <c r="D174" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E174" s="29"/>
+      <c r="E174" s="33"/>
       <c r="F174" s="7" t="s">
         <v>10</v>
       </c>
@@ -3998,7 +3998,7 @@
       <c r="D175" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E175" s="29"/>
+      <c r="E175" s="33"/>
       <c r="F175" s="7" t="s">
         <v>10</v>
       </c>
@@ -4018,7 +4018,7 @@
       <c r="D176" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E176" s="29"/>
+      <c r="E176" s="33"/>
       <c r="F176" s="7" t="s">
         <v>10</v>
       </c>
@@ -4038,7 +4038,7 @@
       <c r="D177" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E177" s="29"/>
+      <c r="E177" s="33"/>
       <c r="F177" s="7" t="s">
         <v>10</v>
       </c>
@@ -4058,7 +4058,7 @@
       <c r="D178" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E178" s="29"/>
+      <c r="E178" s="33"/>
       <c r="F178" s="7" t="s">
         <v>10</v>
       </c>
@@ -4078,7 +4078,7 @@
       <c r="D179" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E179" s="29"/>
+      <c r="E179" s="33"/>
       <c r="F179" s="7" t="s">
         <v>10</v>
       </c>
@@ -4098,7 +4098,7 @@
       <c r="D180" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E180" s="29"/>
+      <c r="E180" s="33"/>
       <c r="F180" s="7" t="s">
         <v>10</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="D181" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E181" s="29"/>
+      <c r="E181" s="33"/>
       <c r="F181" s="7" t="s">
         <v>10</v>
       </c>
@@ -4138,7 +4138,7 @@
       <c r="D182" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E182" s="29"/>
+      <c r="E182" s="33"/>
       <c r="F182" s="7" t="s">
         <v>10</v>
       </c>
@@ -4158,7 +4158,7 @@
       <c r="D183" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E183" s="29"/>
+      <c r="E183" s="33"/>
       <c r="F183" s="7" t="s">
         <v>10</v>
       </c>

</xml_diff>